<commit_message>
file excel dijadikan accounting
</commit_message>
<xml_diff>
--- a/excel/format.xlsx
+++ b/excel/format.xlsx
@@ -45,6 +45,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="42" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,6 +121,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +436,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -433,7 +444,8 @@
     <col min="1" max="1" width="18.875" customWidth="1"/>
     <col min="2" max="2" width="35.625" customWidth="1"/>
     <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="63.75" customWidth="1"/>
+    <col min="4" max="4" width="63.75" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -446,18 +458,19 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>